<commit_message>
CORREÇÃO AO LIMPAR SIGLA
</commit_message>
<xml_diff>
--- a/Producao/Modelos/PERMISSAO_TRABALHO.xlsx
+++ b/Producao/Modelos/PERMISSAO_TRABALHO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wesley\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Servidor\pro_24\Santiago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BAB7254-265D-4365-A889-F61A126D5FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771EC57E-7797-46DA-898E-5C8072F06A77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-15" windowWidth="38640" windowHeight="15720" xr2:uid="{5CC2D26B-3B48-447D-BCE0-CC2304B00E03}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5CC2D26B-3B48-447D-BCE0-CC2304B00E03}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -756,7 +756,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -946,26 +946,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -985,9 +970,348 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -997,356 +1321,8 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4955,6 +4931,80 @@
         <a:xfrm>
           <a:off x="2876550" y="885825"/>
           <a:ext cx="638175" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>638175</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29B0E709-EF2B-A6EB-2888-A9F58161D5D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="51889"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2590800" y="22745700"/>
+          <a:ext cx="2133600" cy="390525"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5393,8 +5443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{825E1A5D-25BB-49A1-A9B6-3D518A8B2BDD}">
   <dimension ref="A1:L105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="G109" sqref="G109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5407,134 +5457,134 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="e" vm="1">
+      <c r="A1" s="83" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="13"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="85"/>
     </row>
     <row r="2" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="127" t="s">
+      <c r="B2" s="87"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="125"/>
-      <c r="H2" s="125"/>
-      <c r="I2" s="125"/>
-      <c r="J2" s="125"/>
-      <c r="K2" s="125"/>
-      <c r="L2" s="126"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="91"/>
     </row>
     <row r="3" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="17" t="s">
+      <c r="B3" s="91"/>
+      <c r="C3" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="17" t="s">
+      <c r="D3" s="90"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="17" t="s">
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="18"/>
-      <c r="L3" s="19"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="91"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="121" t="s">
+      <c r="A4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="31" t="e" vm="2">
+      <c r="B4" s="92"/>
+      <c r="C4" s="93"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="101" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="H4" s="32"/>
-      <c r="I4" s="31" t="e" vm="3">
+      <c r="H4" s="102"/>
+      <c r="I4" s="101" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
-      <c r="J4" s="37"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="40" t="e" vm="4">
+      <c r="J4" s="107"/>
+      <c r="K4" s="102"/>
+      <c r="L4" s="110" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="122"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="41"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="95"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="103"/>
+      <c r="F5" s="104"/>
+      <c r="G5" s="103"/>
+      <c r="H5" s="104"/>
+      <c r="I5" s="103"/>
+      <c r="J5" s="108"/>
+      <c r="K5" s="104"/>
+      <c r="L5" s="111"/>
     </row>
     <row r="6" spans="1:12" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="123"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="42"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="98"/>
+      <c r="C6" s="99"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="105"/>
+      <c r="F6" s="106"/>
+      <c r="G6" s="105"/>
+      <c r="H6" s="106"/>
+      <c r="I6" s="105"/>
+      <c r="J6" s="109"/>
+      <c r="K6" s="106"/>
+      <c r="L6" s="112"/>
     </row>
     <row r="7" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="113" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="43" t="s">
+      <c r="C7" s="114"/>
+      <c r="D7" s="115"/>
+      <c r="E7" s="113" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="45"/>
-      <c r="G7" s="43" t="s">
+      <c r="F7" s="115"/>
+      <c r="G7" s="113" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="45"/>
-      <c r="I7" s="43" t="s">
+      <c r="H7" s="115"/>
+      <c r="I7" s="113" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="44"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="49" t="s">
+      <c r="J7" s="114"/>
+      <c r="K7" s="115"/>
+      <c r="L7" s="119" t="s">
         <v>15</v>
       </c>
     </row>
@@ -5542,1677 +5592,1677 @@
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="46"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="46" t="s">
+      <c r="B8" s="116"/>
+      <c r="C8" s="117"/>
+      <c r="D8" s="118"/>
+      <c r="E8" s="116" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="48"/>
-      <c r="G8" s="46" t="s">
+      <c r="F8" s="118"/>
+      <c r="G8" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="48"/>
-      <c r="I8" s="46" t="s">
+      <c r="H8" s="118"/>
+      <c r="I8" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="47"/>
-      <c r="K8" s="48"/>
-      <c r="L8" s="50"/>
+      <c r="J8" s="117"/>
+      <c r="K8" s="118"/>
+      <c r="L8" s="120"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="57"/>
-      <c r="B9" s="60"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="69" t="s">
+      <c r="A9" s="62"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="70"/>
-      <c r="I9" s="70"/>
-      <c r="J9" s="71"/>
-      <c r="K9" s="69" t="s">
+      <c r="H9" s="75"/>
+      <c r="I9" s="75"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="L9" s="71"/>
+      <c r="L9" s="76"/>
     </row>
     <row r="10" spans="1:12" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="58"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="65"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="72"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
-      <c r="J10" s="74"/>
-      <c r="K10" s="72"/>
-      <c r="L10" s="74"/>
+      <c r="A10" s="63"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="77"/>
+      <c r="H10" s="78"/>
+      <c r="I10" s="78"/>
+      <c r="J10" s="79"/>
+      <c r="K10" s="77"/>
+      <c r="L10" s="79"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="58"/>
-      <c r="B11" s="63"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="72"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="73"/>
-      <c r="J11" s="74"/>
-      <c r="K11" s="72"/>
-      <c r="L11" s="74"/>
+      <c r="A11" s="63"/>
+      <c r="B11" s="68"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="77"/>
+      <c r="H11" s="78"/>
+      <c r="I11" s="78"/>
+      <c r="J11" s="79"/>
+      <c r="K11" s="77"/>
+      <c r="L11" s="79"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="58"/>
-      <c r="B12" s="63"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="65"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="65"/>
-      <c r="G12" s="75"/>
-      <c r="H12" s="76"/>
-      <c r="I12" s="76"/>
-      <c r="J12" s="77"/>
-      <c r="K12" s="75"/>
-      <c r="L12" s="77"/>
+      <c r="A12" s="63"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="80"/>
+      <c r="H12" s="81"/>
+      <c r="I12" s="81"/>
+      <c r="J12" s="82"/>
+      <c r="K12" s="80"/>
+      <c r="L12" s="82"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="58"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="65"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="60" t="s">
+      <c r="A13" s="63"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="61"/>
-      <c r="I13" s="61"/>
-      <c r="J13" s="62"/>
-      <c r="K13" s="60" t="s">
+      <c r="H13" s="66"/>
+      <c r="I13" s="66"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="L13" s="62"/>
+      <c r="L13" s="67"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="58"/>
-      <c r="B14" s="63"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="55"/>
-      <c r="I14" s="55"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="56"/>
+      <c r="A14" s="63"/>
+      <c r="B14" s="68"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="9"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="58"/>
-      <c r="B15" s="63"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="54" t="s">
+      <c r="A15" s="63"/>
+      <c r="B15" s="68"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H15" s="55"/>
-      <c r="I15" s="55"/>
-      <c r="J15" s="56"/>
-      <c r="K15" s="54" t="s">
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L15" s="56"/>
+      <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="58"/>
-      <c r="B16" s="63"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="55"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="63"/>
-      <c r="L16" s="65"/>
+      <c r="A16" s="63"/>
+      <c r="B16" s="68"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="68"/>
+      <c r="F16" s="70"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="68"/>
+      <c r="L16" s="70"/>
     </row>
     <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="59"/>
-      <c r="B17" s="66"/>
-      <c r="C17" s="67"/>
-      <c r="D17" s="68"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="68"/>
-      <c r="G17" s="78" t="s">
+      <c r="A17" s="64"/>
+      <c r="B17" s="71"/>
+      <c r="C17" s="72"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="73"/>
+      <c r="G17" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="H17" s="79"/>
-      <c r="I17" s="79"/>
-      <c r="J17" s="80"/>
-      <c r="K17" s="66"/>
-      <c r="L17" s="68"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="71"/>
+      <c r="L17" s="73"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
-      <c r="B18" s="43"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="87" t="s">
+      <c r="B18" s="113"/>
+      <c r="C18" s="114"/>
+      <c r="D18" s="115"/>
+      <c r="E18" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="89"/>
-      <c r="G18" s="99" t="s">
+      <c r="F18" s="26"/>
+      <c r="G18" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="H18" s="100"/>
-      <c r="I18" s="100"/>
-      <c r="J18" s="100"/>
-      <c r="K18" s="100"/>
-      <c r="L18" s="101"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="45"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="46"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="90" t="s">
+      <c r="B19" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="91"/>
-      <c r="D19" s="92"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="102"/>
-      <c r="H19" s="103"/>
-      <c r="I19" s="103"/>
-      <c r="J19" s="103"/>
-      <c r="K19" s="103"/>
-      <c r="L19" s="104"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
+      <c r="K19" s="48"/>
+      <c r="L19" s="49"/>
     </row>
     <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
-      <c r="B20" s="93" t="s">
+      <c r="B20" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="94"/>
-      <c r="D20" s="95"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="105"/>
-      <c r="H20" s="106"/>
-      <c r="I20" s="106"/>
-      <c r="J20" s="106"/>
-      <c r="K20" s="106"/>
-      <c r="L20" s="107"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="52"/>
     </row>
     <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
-      <c r="B21" s="96"/>
-      <c r="C21" s="97"/>
-      <c r="D21" s="98"/>
-      <c r="E21" s="78"/>
-      <c r="F21" s="80"/>
-      <c r="G21" s="108"/>
-      <c r="H21" s="109"/>
-      <c r="I21" s="109"/>
-      <c r="J21" s="109"/>
-      <c r="K21" s="109"/>
-      <c r="L21" s="110"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="54"/>
+      <c r="I21" s="54"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="55"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="81" t="s">
+      <c r="A22" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="82"/>
-      <c r="C22" s="82"/>
-      <c r="D22" s="82"/>
-      <c r="E22" s="83"/>
-      <c r="F22" s="81" t="s">
+      <c r="B22" s="57"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="G22" s="82"/>
-      <c r="H22" s="82"/>
-      <c r="I22" s="82"/>
-      <c r="J22" s="82"/>
-      <c r="K22" s="82"/>
-      <c r="L22" s="83"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="57"/>
+      <c r="I22" s="57"/>
+      <c r="J22" s="57"/>
+      <c r="K22" s="57"/>
+      <c r="L22" s="58"/>
     </row>
     <row r="23" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="84"/>
-      <c r="B23" s="85"/>
-      <c r="C23" s="85"/>
-      <c r="D23" s="85"/>
-      <c r="E23" s="86"/>
-      <c r="F23" s="84"/>
-      <c r="G23" s="85"/>
-      <c r="H23" s="85"/>
-      <c r="I23" s="85"/>
-      <c r="J23" s="85"/>
-      <c r="K23" s="85"/>
-      <c r="L23" s="86"/>
+      <c r="A23" s="59"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="60"/>
+      <c r="I23" s="60"/>
+      <c r="J23" s="60"/>
+      <c r="K23" s="60"/>
+      <c r="L23" s="61"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="81" t="s">
+      <c r="A24" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="82"/>
-      <c r="C24" s="82"/>
-      <c r="D24" s="82"/>
-      <c r="E24" s="83"/>
-      <c r="F24" s="81" t="s">
+      <c r="B24" s="57"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="G24" s="82"/>
-      <c r="H24" s="82"/>
-      <c r="I24" s="82"/>
-      <c r="J24" s="82"/>
-      <c r="K24" s="82"/>
-      <c r="L24" s="83"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="57"/>
+      <c r="J24" s="57"/>
+      <c r="K24" s="57"/>
+      <c r="L24" s="58"/>
     </row>
     <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="84"/>
-      <c r="B25" s="85"/>
-      <c r="C25" s="85"/>
-      <c r="D25" s="85"/>
-      <c r="E25" s="86"/>
-      <c r="F25" s="84"/>
-      <c r="G25" s="85"/>
-      <c r="H25" s="85"/>
-      <c r="I25" s="85"/>
-      <c r="J25" s="85"/>
-      <c r="K25" s="85"/>
-      <c r="L25" s="86"/>
+      <c r="A25" s="59"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="60"/>
+      <c r="I25" s="60"/>
+      <c r="J25" s="60"/>
+      <c r="K25" s="60"/>
+      <c r="L25" s="61"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="81" t="s">
+      <c r="A26" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="82"/>
-      <c r="C26" s="82"/>
-      <c r="D26" s="82"/>
-      <c r="E26" s="82"/>
-      <c r="F26" s="82"/>
-      <c r="G26" s="82"/>
-      <c r="H26" s="82"/>
-      <c r="I26" s="82"/>
-      <c r="J26" s="82"/>
-      <c r="K26" s="82"/>
-      <c r="L26" s="83"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="57"/>
+      <c r="J26" s="57"/>
+      <c r="K26" s="57"/>
+      <c r="L26" s="58"/>
     </row>
     <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="84"/>
-      <c r="B27" s="85"/>
-      <c r="C27" s="85"/>
-      <c r="D27" s="85"/>
-      <c r="E27" s="85"/>
-      <c r="F27" s="85"/>
-      <c r="G27" s="85"/>
-      <c r="H27" s="85"/>
-      <c r="I27" s="85"/>
-      <c r="J27" s="85"/>
-      <c r="K27" s="85"/>
-      <c r="L27" s="86"/>
+      <c r="A27" s="59"/>
+      <c r="B27" s="60"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="60"/>
+      <c r="I27" s="60"/>
+      <c r="J27" s="60"/>
+      <c r="K27" s="60"/>
+      <c r="L27" s="61"/>
     </row>
     <row r="28" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="51" t="s">
+      <c r="A28" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="52"/>
-      <c r="C28" s="52"/>
-      <c r="D28" s="52"/>
-      <c r="E28" s="52"/>
-      <c r="F28" s="52"/>
-      <c r="G28" s="52"/>
-      <c r="H28" s="52"/>
-      <c r="I28" s="52"/>
-      <c r="J28" s="52"/>
-      <c r="K28" s="52"/>
-      <c r="L28" s="53"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="23"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="87" t="s">
+      <c r="A29" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="88"/>
-      <c r="C29" s="88"/>
-      <c r="D29" s="88" t="s">
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="E29" s="88"/>
-      <c r="F29" s="88"/>
-      <c r="G29" s="88"/>
-      <c r="H29" s="88" t="s">
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="I29" s="88"/>
-      <c r="J29" s="88"/>
-      <c r="K29" s="88"/>
-      <c r="L29" s="89"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
+      <c r="K29" s="25"/>
+      <c r="L29" s="26"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="54" t="s">
+      <c r="A30" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="55"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="55" t="s">
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E30" s="55"/>
-      <c r="F30" s="55"/>
-      <c r="G30" s="55"/>
-      <c r="H30" s="55" t="s">
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="I30" s="55"/>
-      <c r="J30" s="55"/>
-      <c r="K30" s="55"/>
-      <c r="L30" s="56"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="9"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="54" t="s">
+      <c r="A31" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="55"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="55" t="s">
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E31" s="55"/>
-      <c r="F31" s="55"/>
-      <c r="G31" s="55"/>
-      <c r="H31" s="55" t="s">
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="I31" s="55"/>
-      <c r="J31" s="55"/>
-      <c r="K31" s="55"/>
-      <c r="L31" s="56"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="9"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="54" t="s">
+      <c r="A32" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="55"/>
-      <c r="C32" s="55"/>
-      <c r="D32" s="55" t="s">
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="55"/>
-      <c r="F32" s="55"/>
-      <c r="G32" s="55"/>
-      <c r="H32" s="55" t="s">
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="I32" s="55"/>
-      <c r="J32" s="55"/>
-      <c r="K32" s="55"/>
-      <c r="L32" s="56"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="9"/>
     </row>
     <row r="33" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="54" t="s">
+      <c r="A33" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="55"/>
-      <c r="C33" s="55"/>
-      <c r="D33" s="55" t="s">
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E33" s="55"/>
-      <c r="F33" s="55"/>
-      <c r="G33" s="55"/>
-      <c r="H33" s="55" t="s">
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="I33" s="55"/>
-      <c r="J33" s="55"/>
-      <c r="K33" s="55"/>
-      <c r="L33" s="56"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="9"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="54" t="s">
+      <c r="A34" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="55"/>
-      <c r="C34" s="55"/>
-      <c r="D34" s="55" t="s">
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E34" s="55"/>
-      <c r="F34" s="55"/>
-      <c r="G34" s="55"/>
-      <c r="H34" s="55" t="s">
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="I34" s="55"/>
-      <c r="J34" s="55"/>
-      <c r="K34" s="55"/>
-      <c r="L34" s="56"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="9"/>
     </row>
     <row r="35" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="54" t="s">
+      <c r="A35" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B35" s="55"/>
-      <c r="C35" s="55"/>
-      <c r="D35" s="55" t="s">
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E35" s="55"/>
-      <c r="F35" s="55"/>
-      <c r="G35" s="55"/>
-      <c r="H35" s="55" t="s">
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="I35" s="55"/>
-      <c r="J35" s="55"/>
-      <c r="K35" s="55"/>
-      <c r="L35" s="56"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="9"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="54" t="s">
+      <c r="A36" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="55"/>
-      <c r="C36" s="55"/>
-      <c r="D36" s="55" t="s">
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E36" s="55"/>
-      <c r="F36" s="55"/>
-      <c r="G36" s="55"/>
-      <c r="H36" s="55" t="s">
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="I36" s="55"/>
-      <c r="J36" s="55"/>
-      <c r="K36" s="55"/>
-      <c r="L36" s="56"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="9"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="54" t="s">
+      <c r="A37" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B37" s="55"/>
-      <c r="C37" s="55"/>
-      <c r="D37" s="55" t="s">
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E37" s="55"/>
-      <c r="F37" s="55"/>
-      <c r="G37" s="55"/>
-      <c r="H37" s="55" t="s">
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="I37" s="55"/>
-      <c r="J37" s="55"/>
-      <c r="K37" s="55"/>
-      <c r="L37" s="56"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="9"/>
     </row>
     <row r="38" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="54" t="s">
+      <c r="A38" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B38" s="55"/>
-      <c r="C38" s="55"/>
-      <c r="D38" s="55" t="s">
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E38" s="55"/>
-      <c r="F38" s="55"/>
-      <c r="G38" s="55"/>
-      <c r="H38" s="55" t="s">
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="I38" s="55"/>
-      <c r="J38" s="55"/>
-      <c r="K38" s="55"/>
-      <c r="L38" s="56"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="9"/>
     </row>
     <row r="39" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="54" t="s">
+      <c r="A39" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B39" s="55"/>
-      <c r="C39" s="55"/>
-      <c r="D39" s="55" t="s">
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E39" s="55"/>
-      <c r="F39" s="55"/>
-      <c r="G39" s="55"/>
-      <c r="H39" s="55" t="s">
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="I39" s="55"/>
-      <c r="J39" s="55"/>
-      <c r="K39" s="55"/>
-      <c r="L39" s="56"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="9"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="54" t="s">
+      <c r="A40" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B40" s="55"/>
-      <c r="C40" s="55"/>
-      <c r="D40" s="116"/>
-      <c r="E40" s="116"/>
-      <c r="F40" s="116"/>
-      <c r="G40" s="116"/>
-      <c r="H40" s="55" t="s">
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="34"/>
+      <c r="G40" s="34"/>
+      <c r="H40" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="I40" s="55"/>
-      <c r="J40" s="55"/>
-      <c r="K40" s="55"/>
-      <c r="L40" s="56"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="9"/>
     </row>
     <row r="41" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="111"/>
-      <c r="B41" s="112"/>
-      <c r="C41" s="112"/>
-      <c r="D41" s="79"/>
-      <c r="E41" s="79"/>
-      <c r="F41" s="79"/>
-      <c r="G41" s="79"/>
-      <c r="H41" s="79"/>
-      <c r="I41" s="79"/>
-      <c r="J41" s="79"/>
-      <c r="K41" s="79"/>
-      <c r="L41" s="80"/>
+      <c r="A41" s="29"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
+      <c r="L41" s="20"/>
     </row>
     <row r="42" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="51" t="s">
+      <c r="A42" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="B42" s="52"/>
-      <c r="C42" s="52"/>
-      <c r="D42" s="52"/>
-      <c r="E42" s="52"/>
-      <c r="F42" s="52"/>
-      <c r="G42" s="52"/>
-      <c r="H42" s="52"/>
-      <c r="I42" s="52"/>
-      <c r="J42" s="52"/>
-      <c r="K42" s="52"/>
-      <c r="L42" s="53"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="22"/>
+      <c r="J42" s="22"/>
+      <c r="K42" s="22"/>
+      <c r="L42" s="23"/>
     </row>
     <row r="43" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="113" t="s">
+      <c r="A43" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="B43" s="114"/>
-      <c r="C43" s="114"/>
-      <c r="D43" s="114" t="s">
+      <c r="B43" s="32"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="E43" s="114"/>
-      <c r="F43" s="114"/>
-      <c r="G43" s="114"/>
-      <c r="H43" s="114" t="s">
+      <c r="E43" s="32"/>
+      <c r="F43" s="32"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="I43" s="114"/>
-      <c r="J43" s="114"/>
-      <c r="K43" s="114"/>
-      <c r="L43" s="115"/>
+      <c r="I43" s="32"/>
+      <c r="J43" s="32"/>
+      <c r="K43" s="32"/>
+      <c r="L43" s="33"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="87" t="s">
+      <c r="A44" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="B44" s="88"/>
-      <c r="C44" s="88"/>
-      <c r="D44" s="88" t="s">
+      <c r="B44" s="25"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E44" s="88"/>
-      <c r="F44" s="88"/>
-      <c r="G44" s="88"/>
-      <c r="H44" s="119" t="s">
+      <c r="E44" s="25"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="25"/>
+      <c r="H44" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="I44" s="119"/>
-      <c r="J44" s="119"/>
-      <c r="K44" s="119"/>
-      <c r="L44" s="120"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
+      <c r="K44" s="27"/>
+      <c r="L44" s="28"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="54" t="s">
+      <c r="A45" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B45" s="55"/>
-      <c r="C45" s="55"/>
-      <c r="D45" s="55" t="s">
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="E45" s="55"/>
-      <c r="F45" s="55"/>
-      <c r="G45" s="55"/>
-      <c r="H45" s="117" t="s">
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="I45" s="117"/>
-      <c r="J45" s="117"/>
-      <c r="K45" s="117"/>
-      <c r="L45" s="118"/>
+      <c r="I45" s="16"/>
+      <c r="J45" s="16"/>
+      <c r="K45" s="16"/>
+      <c r="L45" s="17"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="54" t="s">
+      <c r="A46" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B46" s="55"/>
-      <c r="C46" s="55"/>
-      <c r="D46" s="55" t="s">
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="E46" s="55"/>
-      <c r="F46" s="55"/>
-      <c r="G46" s="55"/>
-      <c r="H46" s="117" t="s">
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="I46" s="117"/>
-      <c r="J46" s="117"/>
-      <c r="K46" s="117"/>
-      <c r="L46" s="118"/>
+      <c r="I46" s="16"/>
+      <c r="J46" s="16"/>
+      <c r="K46" s="16"/>
+      <c r="L46" s="17"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="54" t="s">
+      <c r="A47" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B47" s="55"/>
-      <c r="C47" s="55"/>
-      <c r="D47" s="55" t="s">
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="E47" s="55"/>
-      <c r="F47" s="55"/>
-      <c r="G47" s="55"/>
-      <c r="H47" s="117" t="s">
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="I47" s="117"/>
-      <c r="J47" s="117"/>
-      <c r="K47" s="117"/>
-      <c r="L47" s="118"/>
+      <c r="I47" s="16"/>
+      <c r="J47" s="16"/>
+      <c r="K47" s="16"/>
+      <c r="L47" s="17"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="54" t="s">
+      <c r="A48" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B48" s="55"/>
-      <c r="C48" s="55"/>
-      <c r="D48" s="55" t="s">
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="E48" s="55"/>
-      <c r="F48" s="55"/>
-      <c r="G48" s="55"/>
-      <c r="H48" s="117" t="s">
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="I48" s="117"/>
-      <c r="J48" s="117"/>
-      <c r="K48" s="117"/>
-      <c r="L48" s="118"/>
+      <c r="I48" s="16"/>
+      <c r="J48" s="16"/>
+      <c r="K48" s="16"/>
+      <c r="L48" s="17"/>
     </row>
     <row r="49" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="54" t="s">
+      <c r="A49" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B49" s="55"/>
-      <c r="C49" s="55"/>
-      <c r="D49" s="55" t="s">
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="E49" s="55"/>
-      <c r="F49" s="55"/>
-      <c r="G49" s="55"/>
-      <c r="H49" s="117" t="s">
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="I49" s="117"/>
-      <c r="J49" s="117"/>
-      <c r="K49" s="117"/>
-      <c r="L49" s="118"/>
+      <c r="I49" s="16"/>
+      <c r="J49" s="16"/>
+      <c r="K49" s="16"/>
+      <c r="L49" s="17"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="54" t="s">
+      <c r="A50" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B50" s="55"/>
-      <c r="C50" s="55"/>
-      <c r="D50" s="55" t="s">
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E50" s="55"/>
-      <c r="F50" s="55"/>
-      <c r="G50" s="55"/>
-      <c r="H50" s="117" t="s">
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="I50" s="117"/>
-      <c r="J50" s="117"/>
-      <c r="K50" s="117"/>
-      <c r="L50" s="118"/>
+      <c r="I50" s="16"/>
+      <c r="J50" s="16"/>
+      <c r="K50" s="16"/>
+      <c r="L50" s="17"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="54" t="s">
+      <c r="A51" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B51" s="55"/>
-      <c r="C51" s="55"/>
-      <c r="D51" s="55" t="s">
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="E51" s="55"/>
-      <c r="F51" s="55"/>
-      <c r="G51" s="55"/>
-      <c r="H51" s="117" t="s">
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="I51" s="117"/>
-      <c r="J51" s="117"/>
-      <c r="K51" s="117"/>
-      <c r="L51" s="118"/>
+      <c r="I51" s="16"/>
+      <c r="J51" s="16"/>
+      <c r="K51" s="16"/>
+      <c r="L51" s="17"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="54" t="s">
+      <c r="A52" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B52" s="55"/>
-      <c r="C52" s="55"/>
-      <c r="D52" s="55" t="s">
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="E52" s="55"/>
-      <c r="F52" s="55"/>
-      <c r="G52" s="55"/>
-      <c r="H52" s="117" t="s">
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="I52" s="117"/>
-      <c r="J52" s="117"/>
-      <c r="K52" s="117"/>
-      <c r="L52" s="118"/>
+      <c r="I52" s="16"/>
+      <c r="J52" s="16"/>
+      <c r="K52" s="16"/>
+      <c r="L52" s="17"/>
     </row>
     <row r="53" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="54" t="s">
+      <c r="A53" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B53" s="55"/>
-      <c r="C53" s="55"/>
-      <c r="D53" s="55" t="s">
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="E53" s="55"/>
-      <c r="F53" s="55"/>
-      <c r="G53" s="55"/>
-      <c r="H53" s="117" t="s">
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="I53" s="117"/>
-      <c r="J53" s="117"/>
-      <c r="K53" s="117"/>
-      <c r="L53" s="118"/>
+      <c r="I53" s="16"/>
+      <c r="J53" s="16"/>
+      <c r="K53" s="16"/>
+      <c r="L53" s="17"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" s="54" t="s">
+      <c r="A54" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B54" s="55"/>
-      <c r="C54" s="55"/>
-      <c r="D54" s="55" t="s">
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="E54" s="55"/>
-      <c r="F54" s="55"/>
-      <c r="G54" s="55"/>
-      <c r="H54" s="117" t="s">
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="I54" s="117"/>
-      <c r="J54" s="117"/>
-      <c r="K54" s="117"/>
-      <c r="L54" s="118"/>
+      <c r="I54" s="16"/>
+      <c r="J54" s="16"/>
+      <c r="K54" s="16"/>
+      <c r="L54" s="17"/>
     </row>
     <row r="55" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="54" t="s">
+      <c r="A55" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B55" s="55"/>
-      <c r="C55" s="55"/>
-      <c r="D55" s="55" t="s">
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="E55" s="55"/>
-      <c r="F55" s="55"/>
-      <c r="G55" s="55"/>
-      <c r="H55" s="117" t="s">
+      <c r="E55" s="8"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="I55" s="117"/>
-      <c r="J55" s="117"/>
-      <c r="K55" s="117"/>
-      <c r="L55" s="118"/>
+      <c r="I55" s="16"/>
+      <c r="J55" s="16"/>
+      <c r="K55" s="16"/>
+      <c r="L55" s="17"/>
     </row>
     <row r="56" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="54" t="s">
+      <c r="A56" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B56" s="55"/>
-      <c r="C56" s="55"/>
-      <c r="D56" s="55" t="s">
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="E56" s="55"/>
-      <c r="F56" s="55"/>
-      <c r="G56" s="55"/>
-      <c r="H56" s="117" t="s">
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="8"/>
+      <c r="H56" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="I56" s="117"/>
-      <c r="J56" s="117"/>
-      <c r="K56" s="117"/>
-      <c r="L56" s="118"/>
+      <c r="I56" s="16"/>
+      <c r="J56" s="16"/>
+      <c r="K56" s="16"/>
+      <c r="L56" s="17"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" s="54" t="s">
+      <c r="A57" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B57" s="55"/>
-      <c r="C57" s="55"/>
-      <c r="D57" s="55" t="s">
+      <c r="B57" s="8"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="E57" s="55"/>
-      <c r="F57" s="55"/>
-      <c r="G57" s="55"/>
-      <c r="H57" s="55" t="s">
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="I57" s="55"/>
-      <c r="J57" s="55"/>
-      <c r="K57" s="55"/>
-      <c r="L57" s="56"/>
+      <c r="I57" s="8"/>
+      <c r="J57" s="8"/>
+      <c r="K57" s="8"/>
+      <c r="L57" s="9"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="54" t="s">
+      <c r="A58" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B58" s="55"/>
-      <c r="C58" s="55"/>
-      <c r="D58" s="55" t="s">
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="E58" s="55"/>
-      <c r="F58" s="55"/>
-      <c r="G58" s="55"/>
-      <c r="H58" s="55"/>
-      <c r="I58" s="55"/>
-      <c r="J58" s="55"/>
-      <c r="K58" s="55"/>
-      <c r="L58" s="56"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="8"/>
+      <c r="K58" s="8"/>
+      <c r="L58" s="9"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59" s="54" t="s">
+      <c r="A59" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B59" s="55"/>
-      <c r="C59" s="55"/>
-      <c r="D59" s="55" t="s">
+      <c r="B59" s="8"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="E59" s="55"/>
-      <c r="F59" s="55"/>
-      <c r="G59" s="55"/>
-      <c r="H59" s="55"/>
-      <c r="I59" s="55"/>
-      <c r="J59" s="55"/>
-      <c r="K59" s="55"/>
-      <c r="L59" s="56"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="8"/>
+      <c r="I59" s="8"/>
+      <c r="J59" s="8"/>
+      <c r="K59" s="8"/>
+      <c r="L59" s="9"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="54" t="s">
+      <c r="A60" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="B60" s="55"/>
-      <c r="C60" s="55"/>
-      <c r="D60" s="55" t="s">
+      <c r="B60" s="8"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="E60" s="55"/>
-      <c r="F60" s="55"/>
-      <c r="G60" s="55"/>
-      <c r="H60" s="55"/>
-      <c r="I60" s="55"/>
-      <c r="J60" s="55"/>
-      <c r="K60" s="55"/>
-      <c r="L60" s="56"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="8"/>
+      <c r="G60" s="8"/>
+      <c r="H60" s="8"/>
+      <c r="I60" s="8"/>
+      <c r="J60" s="8"/>
+      <c r="K60" s="8"/>
+      <c r="L60" s="9"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A61" s="54" t="s">
+      <c r="A61" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B61" s="55"/>
-      <c r="C61" s="55"/>
-      <c r="D61" s="55" t="s">
+      <c r="B61" s="8"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="E61" s="55"/>
-      <c r="F61" s="55"/>
-      <c r="G61" s="55"/>
-      <c r="H61" s="55"/>
-      <c r="I61" s="55"/>
-      <c r="J61" s="55"/>
-      <c r="K61" s="55"/>
-      <c r="L61" s="56"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="8"/>
+      <c r="G61" s="8"/>
+      <c r="H61" s="8"/>
+      <c r="I61" s="8"/>
+      <c r="J61" s="8"/>
+      <c r="K61" s="8"/>
+      <c r="L61" s="9"/>
     </row>
     <row r="62" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="78"/>
-      <c r="B62" s="79"/>
-      <c r="C62" s="79"/>
-      <c r="D62" s="79"/>
-      <c r="E62" s="79"/>
-      <c r="F62" s="79"/>
-      <c r="G62" s="79"/>
-      <c r="H62" s="79"/>
-      <c r="I62" s="79"/>
-      <c r="J62" s="79"/>
-      <c r="K62" s="79"/>
-      <c r="L62" s="80"/>
+      <c r="A62" s="18"/>
+      <c r="B62" s="19"/>
+      <c r="C62" s="19"/>
+      <c r="D62" s="19"/>
+      <c r="E62" s="19"/>
+      <c r="F62" s="19"/>
+      <c r="G62" s="19"/>
+      <c r="H62" s="19"/>
+      <c r="I62" s="19"/>
+      <c r="J62" s="19"/>
+      <c r="K62" s="19"/>
+      <c r="L62" s="20"/>
     </row>
     <row r="63" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="51" t="s">
+      <c r="A63" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="B63" s="52"/>
-      <c r="C63" s="52"/>
-      <c r="D63" s="52"/>
-      <c r="E63" s="52"/>
-      <c r="F63" s="52"/>
-      <c r="G63" s="52"/>
-      <c r="H63" s="52"/>
-      <c r="I63" s="52"/>
-      <c r="J63" s="52"/>
-      <c r="K63" s="52"/>
-      <c r="L63" s="53"/>
+      <c r="B63" s="22"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="22"/>
+      <c r="F63" s="22"/>
+      <c r="G63" s="22"/>
+      <c r="H63" s="22"/>
+      <c r="I63" s="22"/>
+      <c r="J63" s="22"/>
+      <c r="K63" s="22"/>
+      <c r="L63" s="23"/>
     </row>
     <row r="64" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="87" t="s">
+      <c r="A64" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="B64" s="88"/>
-      <c r="C64" s="88"/>
-      <c r="D64" s="88" t="s">
+      <c r="B64" s="25"/>
+      <c r="C64" s="25"/>
+      <c r="D64" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="E64" s="88"/>
-      <c r="F64" s="88"/>
-      <c r="G64" s="88"/>
-      <c r="H64" s="88" t="s">
+      <c r="E64" s="25"/>
+      <c r="F64" s="25"/>
+      <c r="G64" s="25"/>
+      <c r="H64" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="I64" s="88"/>
-      <c r="J64" s="88"/>
-      <c r="K64" s="88"/>
-      <c r="L64" s="89"/>
+      <c r="I64" s="25"/>
+      <c r="J64" s="25"/>
+      <c r="K64" s="25"/>
+      <c r="L64" s="26"/>
     </row>
     <row r="65" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="54" t="s">
+      <c r="A65" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="B65" s="55"/>
-      <c r="C65" s="55"/>
-      <c r="D65" s="55" t="s">
+      <c r="B65" s="8"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="E65" s="55"/>
-      <c r="F65" s="55"/>
-      <c r="G65" s="55"/>
-      <c r="H65" s="55" t="s">
+      <c r="E65" s="8"/>
+      <c r="F65" s="8"/>
+      <c r="G65" s="8"/>
+      <c r="H65" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="I65" s="55"/>
-      <c r="J65" s="55"/>
-      <c r="K65" s="55"/>
-      <c r="L65" s="56"/>
+      <c r="I65" s="8"/>
+      <c r="J65" s="8"/>
+      <c r="K65" s="8"/>
+      <c r="L65" s="9"/>
     </row>
     <row r="66" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="54" t="s">
+      <c r="A66" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B66" s="55"/>
-      <c r="C66" s="55"/>
-      <c r="D66" s="55" t="s">
+      <c r="B66" s="8"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="E66" s="55"/>
-      <c r="F66" s="55"/>
-      <c r="G66" s="55"/>
-      <c r="H66" s="117" t="s">
+      <c r="E66" s="8"/>
+      <c r="F66" s="8"/>
+      <c r="G66" s="8"/>
+      <c r="H66" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="I66" s="117"/>
-      <c r="J66" s="117"/>
-      <c r="K66" s="117"/>
-      <c r="L66" s="118"/>
+      <c r="I66" s="16"/>
+      <c r="J66" s="16"/>
+      <c r="K66" s="16"/>
+      <c r="L66" s="17"/>
     </row>
     <row r="67" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="54" t="s">
+      <c r="A67" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="B67" s="55"/>
-      <c r="C67" s="55"/>
-      <c r="D67" s="55" t="s">
+      <c r="B67" s="8"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="E67" s="55"/>
-      <c r="F67" s="55"/>
-      <c r="G67" s="55"/>
-      <c r="H67" s="117" t="s">
+      <c r="E67" s="8"/>
+      <c r="F67" s="8"/>
+      <c r="G67" s="8"/>
+      <c r="H67" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="I67" s="117"/>
-      <c r="J67" s="117"/>
-      <c r="K67" s="117"/>
-      <c r="L67" s="118"/>
+      <c r="I67" s="16"/>
+      <c r="J67" s="16"/>
+      <c r="K67" s="16"/>
+      <c r="L67" s="17"/>
     </row>
     <row r="68" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="54" t="s">
+      <c r="A68" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="B68" s="55"/>
-      <c r="C68" s="55"/>
-      <c r="D68" s="55" t="s">
+      <c r="B68" s="8"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="E68" s="55"/>
-      <c r="F68" s="55"/>
-      <c r="G68" s="55"/>
-      <c r="H68" s="55" t="s">
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="8"/>
+      <c r="H68" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="I68" s="55"/>
-      <c r="J68" s="55"/>
-      <c r="K68" s="55"/>
-      <c r="L68" s="56"/>
+      <c r="I68" s="8"/>
+      <c r="J68" s="8"/>
+      <c r="K68" s="8"/>
+      <c r="L68" s="9"/>
     </row>
     <row r="69" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="54" t="s">
+      <c r="A69" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="B69" s="55"/>
-      <c r="C69" s="55"/>
-      <c r="D69" s="55" t="s">
+      <c r="B69" s="8"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="E69" s="55"/>
-      <c r="F69" s="55"/>
-      <c r="G69" s="55"/>
-      <c r="H69" s="55" t="s">
+      <c r="E69" s="8"/>
+      <c r="F69" s="8"/>
+      <c r="G69" s="8"/>
+      <c r="H69" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="I69" s="55"/>
-      <c r="J69" s="55"/>
-      <c r="K69" s="55"/>
-      <c r="L69" s="56"/>
+      <c r="I69" s="8"/>
+      <c r="J69" s="8"/>
+      <c r="K69" s="8"/>
+      <c r="L69" s="9"/>
     </row>
     <row r="70" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="54" t="s">
+      <c r="A70" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="B70" s="55"/>
-      <c r="C70" s="55"/>
-      <c r="D70" s="55" t="s">
+      <c r="B70" s="8"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="E70" s="55"/>
-      <c r="F70" s="55"/>
-      <c r="G70" s="55"/>
-      <c r="H70" s="55" t="s">
+      <c r="E70" s="8"/>
+      <c r="F70" s="8"/>
+      <c r="G70" s="8"/>
+      <c r="H70" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="I70" s="55"/>
-      <c r="J70" s="55"/>
-      <c r="K70" s="55"/>
-      <c r="L70" s="56"/>
+      <c r="I70" s="8"/>
+      <c r="J70" s="8"/>
+      <c r="K70" s="8"/>
+      <c r="L70" s="9"/>
     </row>
     <row r="71" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="54" t="s">
+      <c r="A71" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="B71" s="55"/>
-      <c r="C71" s="55"/>
-      <c r="D71" s="55" t="s">
+      <c r="B71" s="8"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="E71" s="55"/>
-      <c r="F71" s="55"/>
-      <c r="G71" s="55"/>
-      <c r="H71" s="55" t="s">
+      <c r="E71" s="8"/>
+      <c r="F71" s="8"/>
+      <c r="G71" s="8"/>
+      <c r="H71" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="I71" s="55"/>
-      <c r="J71" s="55"/>
-      <c r="K71" s="55"/>
-      <c r="L71" s="56"/>
+      <c r="I71" s="8"/>
+      <c r="J71" s="8"/>
+      <c r="K71" s="8"/>
+      <c r="L71" s="9"/>
     </row>
     <row r="72" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="54" t="s">
+      <c r="A72" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="B72" s="55"/>
-      <c r="C72" s="55"/>
-      <c r="D72" s="55" t="s">
+      <c r="B72" s="8"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="E72" s="55"/>
-      <c r="F72" s="55"/>
-      <c r="G72" s="55"/>
-      <c r="H72" s="55" t="s">
+      <c r="E72" s="8"/>
+      <c r="F72" s="8"/>
+      <c r="G72" s="8"/>
+      <c r="H72" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="I72" s="55"/>
-      <c r="J72" s="55"/>
-      <c r="K72" s="55"/>
-      <c r="L72" s="56"/>
+      <c r="I72" s="8"/>
+      <c r="J72" s="8"/>
+      <c r="K72" s="8"/>
+      <c r="L72" s="9"/>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A73" s="54" t="s">
+      <c r="A73" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="B73" s="55"/>
-      <c r="C73" s="55"/>
-      <c r="D73" s="117" t="s">
+      <c r="B73" s="8"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="E73" s="117"/>
-      <c r="F73" s="117"/>
-      <c r="G73" s="117"/>
-      <c r="H73" s="55" t="s">
+      <c r="E73" s="16"/>
+      <c r="F73" s="16"/>
+      <c r="G73" s="16"/>
+      <c r="H73" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="I73" s="55"/>
-      <c r="J73" s="55"/>
-      <c r="K73" s="55"/>
-      <c r="L73" s="56"/>
+      <c r="I73" s="8"/>
+      <c r="J73" s="8"/>
+      <c r="K73" s="8"/>
+      <c r="L73" s="9"/>
     </row>
     <row r="74" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="54" t="s">
+      <c r="A74" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="B74" s="55"/>
-      <c r="C74" s="55"/>
-      <c r="D74" s="117" t="s">
+      <c r="B74" s="8"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="E74" s="117"/>
-      <c r="F74" s="117"/>
-      <c r="G74" s="117"/>
-      <c r="H74" s="55" t="s">
+      <c r="E74" s="16"/>
+      <c r="F74" s="16"/>
+      <c r="G74" s="16"/>
+      <c r="H74" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="I74" s="55"/>
-      <c r="J74" s="55"/>
-      <c r="K74" s="55"/>
-      <c r="L74" s="56"/>
+      <c r="I74" s="8"/>
+      <c r="J74" s="8"/>
+      <c r="K74" s="8"/>
+      <c r="L74" s="9"/>
     </row>
     <row r="75" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="54" t="s">
+      <c r="A75" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="B75" s="55"/>
-      <c r="C75" s="55"/>
-      <c r="D75" s="117" t="s">
+      <c r="B75" s="8"/>
+      <c r="C75" s="8"/>
+      <c r="D75" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="E75" s="117"/>
-      <c r="F75" s="117"/>
-      <c r="G75" s="117"/>
-      <c r="H75" s="55" t="s">
+      <c r="E75" s="16"/>
+      <c r="F75" s="16"/>
+      <c r="G75" s="16"/>
+      <c r="H75" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="I75" s="55"/>
-      <c r="J75" s="55"/>
-      <c r="K75" s="55"/>
-      <c r="L75" s="56"/>
+      <c r="I75" s="8"/>
+      <c r="J75" s="8"/>
+      <c r="K75" s="8"/>
+      <c r="L75" s="9"/>
     </row>
     <row r="76" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="54" t="s">
+      <c r="A76" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="B76" s="55"/>
-      <c r="C76" s="55"/>
-      <c r="D76" s="117" t="s">
+      <c r="B76" s="8"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="E76" s="117"/>
-      <c r="F76" s="117"/>
-      <c r="G76" s="117"/>
-      <c r="H76" s="55"/>
-      <c r="I76" s="55"/>
-      <c r="J76" s="55"/>
-      <c r="K76" s="55"/>
-      <c r="L76" s="56"/>
+      <c r="E76" s="16"/>
+      <c r="F76" s="16"/>
+      <c r="G76" s="16"/>
+      <c r="H76" s="8"/>
+      <c r="I76" s="8"/>
+      <c r="J76" s="8"/>
+      <c r="K76" s="8"/>
+      <c r="L76" s="9"/>
     </row>
     <row r="77" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="54" t="s">
+      <c r="A77" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="B77" s="55"/>
-      <c r="C77" s="55"/>
-      <c r="D77" s="55" t="s">
+      <c r="B77" s="8"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="E77" s="55"/>
-      <c r="F77" s="55"/>
-      <c r="G77" s="55"/>
-      <c r="H77" s="55"/>
-      <c r="I77" s="55"/>
-      <c r="J77" s="55"/>
-      <c r="K77" s="55"/>
-      <c r="L77" s="56"/>
+      <c r="E77" s="8"/>
+      <c r="F77" s="8"/>
+      <c r="G77" s="8"/>
+      <c r="H77" s="8"/>
+      <c r="I77" s="8"/>
+      <c r="J77" s="8"/>
+      <c r="K77" s="8"/>
+      <c r="L77" s="9"/>
     </row>
     <row r="78" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="54" t="s">
+      <c r="A78" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="B78" s="55"/>
-      <c r="C78" s="55"/>
-      <c r="D78" s="55" t="s">
+      <c r="B78" s="8"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="E78" s="55"/>
-      <c r="F78" s="55"/>
-      <c r="G78" s="55"/>
-      <c r="H78" s="55"/>
-      <c r="I78" s="55"/>
-      <c r="J78" s="55"/>
-      <c r="K78" s="55"/>
-      <c r="L78" s="56"/>
+      <c r="E78" s="8"/>
+      <c r="F78" s="8"/>
+      <c r="G78" s="8"/>
+      <c r="H78" s="8"/>
+      <c r="I78" s="8"/>
+      <c r="J78" s="8"/>
+      <c r="K78" s="8"/>
+      <c r="L78" s="9"/>
     </row>
     <row r="79" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="54" t="s">
+      <c r="A79" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="B79" s="55"/>
-      <c r="C79" s="55"/>
-      <c r="D79" s="55" t="s">
+      <c r="B79" s="8"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="E79" s="55"/>
-      <c r="F79" s="55"/>
-      <c r="G79" s="55"/>
-      <c r="H79" s="55"/>
-      <c r="I79" s="55"/>
-      <c r="J79" s="55"/>
-      <c r="K79" s="55"/>
-      <c r="L79" s="56"/>
+      <c r="E79" s="8"/>
+      <c r="F79" s="8"/>
+      <c r="G79" s="8"/>
+      <c r="H79" s="8"/>
+      <c r="I79" s="8"/>
+      <c r="J79" s="8"/>
+      <c r="K79" s="8"/>
+      <c r="L79" s="9"/>
     </row>
     <row r="80" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="54" t="s">
+      <c r="A80" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="B80" s="55"/>
-      <c r="C80" s="55"/>
-      <c r="D80" s="55" t="s">
+      <c r="B80" s="8"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="E80" s="55"/>
-      <c r="F80" s="55"/>
-      <c r="G80" s="55"/>
-      <c r="H80" s="55"/>
-      <c r="I80" s="55"/>
-      <c r="J80" s="55"/>
-      <c r="K80" s="55"/>
-      <c r="L80" s="56"/>
+      <c r="E80" s="8"/>
+      <c r="F80" s="8"/>
+      <c r="G80" s="8"/>
+      <c r="H80" s="8"/>
+      <c r="I80" s="8"/>
+      <c r="J80" s="8"/>
+      <c r="K80" s="8"/>
+      <c r="L80" s="9"/>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A81" s="54" t="s">
+      <c r="A81" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="B81" s="55"/>
-      <c r="C81" s="55"/>
-      <c r="D81" s="55" t="s">
+      <c r="B81" s="8"/>
+      <c r="C81" s="8"/>
+      <c r="D81" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="E81" s="55"/>
-      <c r="F81" s="55"/>
-      <c r="G81" s="55"/>
-      <c r="H81" s="55"/>
-      <c r="I81" s="55"/>
-      <c r="J81" s="55"/>
-      <c r="K81" s="55"/>
-      <c r="L81" s="56"/>
+      <c r="E81" s="8"/>
+      <c r="F81" s="8"/>
+      <c r="G81" s="8"/>
+      <c r="H81" s="8"/>
+      <c r="I81" s="8"/>
+      <c r="J81" s="8"/>
+      <c r="K81" s="8"/>
+      <c r="L81" s="9"/>
     </row>
     <row r="82" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="20" t="s">
+      <c r="A82" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="B82" s="20"/>
-      <c r="C82" s="20"/>
-      <c r="D82" s="20" t="s">
+      <c r="B82" s="12"/>
+      <c r="C82" s="12"/>
+      <c r="D82" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="E82" s="20"/>
-      <c r="F82" s="20"/>
-      <c r="G82" s="20"/>
-      <c r="H82" s="20"/>
-      <c r="I82" s="20" t="s">
+      <c r="E82" s="12"/>
+      <c r="F82" s="12"/>
+      <c r="G82" s="12"/>
+      <c r="H82" s="12"/>
+      <c r="I82" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="J82" s="20"/>
-      <c r="K82" s="20"/>
-      <c r="L82" s="20"/>
+      <c r="J82" s="12"/>
+      <c r="K82" s="12"/>
+      <c r="L82" s="12"/>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A83" s="21"/>
-      <c r="B83" s="21"/>
-      <c r="C83" s="21"/>
-      <c r="D83" s="7"/>
-      <c r="E83" s="7"/>
-      <c r="F83" s="7"/>
-      <c r="G83" s="7"/>
-      <c r="H83" s="7"/>
-      <c r="I83" s="7"/>
-      <c r="J83" s="7"/>
-      <c r="K83" s="7"/>
-      <c r="L83" s="7"/>
+      <c r="A83" s="10"/>
+      <c r="B83" s="10"/>
+      <c r="C83" s="10"/>
+      <c r="D83" s="11"/>
+      <c r="E83" s="11"/>
+      <c r="F83" s="11"/>
+      <c r="G83" s="11"/>
+      <c r="H83" s="11"/>
+      <c r="I83" s="11"/>
+      <c r="J83" s="11"/>
+      <c r="K83" s="11"/>
+      <c r="L83" s="11"/>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A84" s="21"/>
-      <c r="B84" s="21"/>
-      <c r="C84" s="21"/>
-      <c r="D84" s="7"/>
-      <c r="E84" s="7"/>
-      <c r="F84" s="7"/>
-      <c r="G84" s="7"/>
-      <c r="H84" s="7"/>
-      <c r="I84" s="7"/>
-      <c r="J84" s="7"/>
-      <c r="K84" s="7"/>
-      <c r="L84" s="7"/>
+      <c r="A84" s="10"/>
+      <c r="B84" s="10"/>
+      <c r="C84" s="10"/>
+      <c r="D84" s="11"/>
+      <c r="E84" s="11"/>
+      <c r="F84" s="11"/>
+      <c r="G84" s="11"/>
+      <c r="H84" s="11"/>
+      <c r="I84" s="11"/>
+      <c r="J84" s="11"/>
+      <c r="K84" s="11"/>
+      <c r="L84" s="11"/>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A85" s="21"/>
-      <c r="B85" s="21"/>
-      <c r="C85" s="21"/>
-      <c r="D85" s="7"/>
-      <c r="E85" s="7"/>
-      <c r="F85" s="7"/>
-      <c r="G85" s="7"/>
-      <c r="H85" s="7"/>
-      <c r="I85" s="7"/>
-      <c r="J85" s="7"/>
-      <c r="K85" s="7"/>
-      <c r="L85" s="7"/>
+      <c r="A85" s="10"/>
+      <c r="B85" s="10"/>
+      <c r="C85" s="10"/>
+      <c r="D85" s="11"/>
+      <c r="E85" s="11"/>
+      <c r="F85" s="11"/>
+      <c r="G85" s="11"/>
+      <c r="H85" s="11"/>
+      <c r="I85" s="11"/>
+      <c r="J85" s="11"/>
+      <c r="K85" s="11"/>
+      <c r="L85" s="11"/>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A86" s="21"/>
-      <c r="B86" s="21"/>
-      <c r="C86" s="21"/>
-      <c r="D86" s="7"/>
-      <c r="E86" s="7"/>
-      <c r="F86" s="7"/>
-      <c r="G86" s="7"/>
-      <c r="H86" s="7"/>
-      <c r="I86" s="7"/>
-      <c r="J86" s="7"/>
-      <c r="K86" s="7"/>
-      <c r="L86" s="7"/>
+      <c r="A86" s="10"/>
+      <c r="B86" s="10"/>
+      <c r="C86" s="10"/>
+      <c r="D86" s="11"/>
+      <c r="E86" s="11"/>
+      <c r="F86" s="11"/>
+      <c r="G86" s="11"/>
+      <c r="H86" s="11"/>
+      <c r="I86" s="11"/>
+      <c r="J86" s="11"/>
+      <c r="K86" s="11"/>
+      <c r="L86" s="11"/>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A87" s="21"/>
-      <c r="B87" s="21"/>
-      <c r="C87" s="21"/>
-      <c r="D87" s="7"/>
-      <c r="E87" s="7"/>
-      <c r="F87" s="7"/>
-      <c r="G87" s="7"/>
-      <c r="H87" s="7"/>
-      <c r="I87" s="7"/>
-      <c r="J87" s="7"/>
-      <c r="K87" s="7"/>
-      <c r="L87" s="7"/>
+      <c r="A87" s="10"/>
+      <c r="B87" s="10"/>
+      <c r="C87" s="10"/>
+      <c r="D87" s="11"/>
+      <c r="E87" s="11"/>
+      <c r="F87" s="11"/>
+      <c r="G87" s="11"/>
+      <c r="H87" s="11"/>
+      <c r="I87" s="11"/>
+      <c r="J87" s="11"/>
+      <c r="K87" s="11"/>
+      <c r="L87" s="11"/>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A88" s="21"/>
-      <c r="B88" s="21"/>
-      <c r="C88" s="21"/>
-      <c r="D88" s="7"/>
-      <c r="E88" s="7"/>
-      <c r="F88" s="7"/>
-      <c r="G88" s="7"/>
-      <c r="H88" s="7"/>
-      <c r="I88" s="7"/>
-      <c r="J88" s="7"/>
-      <c r="K88" s="7"/>
-      <c r="L88" s="7"/>
+      <c r="A88" s="10"/>
+      <c r="B88" s="10"/>
+      <c r="C88" s="10"/>
+      <c r="D88" s="11"/>
+      <c r="E88" s="11"/>
+      <c r="F88" s="11"/>
+      <c r="G88" s="11"/>
+      <c r="H88" s="11"/>
+      <c r="I88" s="11"/>
+      <c r="J88" s="11"/>
+      <c r="K88" s="11"/>
+      <c r="L88" s="11"/>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A89" s="21"/>
-      <c r="B89" s="21"/>
-      <c r="C89" s="21"/>
-      <c r="D89" s="7"/>
-      <c r="E89" s="7"/>
-      <c r="F89" s="7"/>
-      <c r="G89" s="7"/>
-      <c r="H89" s="7"/>
-      <c r="I89" s="7"/>
-      <c r="J89" s="7"/>
-      <c r="K89" s="7"/>
-      <c r="L89" s="7"/>
+      <c r="A89" s="10"/>
+      <c r="B89" s="10"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="11"/>
+      <c r="E89" s="11"/>
+      <c r="F89" s="11"/>
+      <c r="G89" s="11"/>
+      <c r="H89" s="11"/>
+      <c r="I89" s="11"/>
+      <c r="J89" s="11"/>
+      <c r="K89" s="11"/>
+      <c r="L89" s="11"/>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A90" s="21"/>
-      <c r="B90" s="21"/>
-      <c r="C90" s="21"/>
-      <c r="D90" s="7"/>
-      <c r="E90" s="7"/>
-      <c r="F90" s="7"/>
-      <c r="G90" s="7"/>
-      <c r="H90" s="7"/>
-      <c r="I90" s="7"/>
-      <c r="J90" s="7"/>
-      <c r="K90" s="7"/>
-      <c r="L90" s="7"/>
+      <c r="A90" s="10"/>
+      <c r="B90" s="10"/>
+      <c r="C90" s="10"/>
+      <c r="D90" s="11"/>
+      <c r="E90" s="11"/>
+      <c r="F90" s="11"/>
+      <c r="G90" s="11"/>
+      <c r="H90" s="11"/>
+      <c r="I90" s="11"/>
+      <c r="J90" s="11"/>
+      <c r="K90" s="11"/>
+      <c r="L90" s="11"/>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A91" s="21"/>
-      <c r="B91" s="21"/>
-      <c r="C91" s="21"/>
-      <c r="D91" s="7"/>
-      <c r="E91" s="7"/>
-      <c r="F91" s="7"/>
-      <c r="G91" s="7"/>
-      <c r="H91" s="7"/>
-      <c r="I91" s="7"/>
-      <c r="J91" s="7"/>
-      <c r="K91" s="7"/>
-      <c r="L91" s="7"/>
+      <c r="A91" s="10"/>
+      <c r="B91" s="10"/>
+      <c r="C91" s="10"/>
+      <c r="D91" s="11"/>
+      <c r="E91" s="11"/>
+      <c r="F91" s="11"/>
+      <c r="G91" s="11"/>
+      <c r="H91" s="11"/>
+      <c r="I91" s="11"/>
+      <c r="J91" s="11"/>
+      <c r="K91" s="11"/>
+      <c r="L91" s="11"/>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A92" s="21"/>
-      <c r="B92" s="21"/>
-      <c r="C92" s="21"/>
-      <c r="D92" s="7"/>
-      <c r="E92" s="7"/>
-      <c r="F92" s="7"/>
-      <c r="G92" s="7"/>
-      <c r="H92" s="7"/>
-      <c r="I92" s="7"/>
-      <c r="J92" s="7"/>
-      <c r="K92" s="7"/>
-      <c r="L92" s="7"/>
+      <c r="A92" s="10"/>
+      <c r="B92" s="10"/>
+      <c r="C92" s="10"/>
+      <c r="D92" s="11"/>
+      <c r="E92" s="11"/>
+      <c r="F92" s="11"/>
+      <c r="G92" s="11"/>
+      <c r="H92" s="11"/>
+      <c r="I92" s="11"/>
+      <c r="J92" s="11"/>
+      <c r="K92" s="11"/>
+      <c r="L92" s="11"/>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A93" s="21"/>
-      <c r="B93" s="21"/>
-      <c r="C93" s="21"/>
-      <c r="D93" s="7"/>
-      <c r="E93" s="7"/>
-      <c r="F93" s="7"/>
-      <c r="G93" s="7"/>
-      <c r="H93" s="7"/>
-      <c r="I93" s="7"/>
-      <c r="J93" s="7"/>
-      <c r="K93" s="7"/>
-      <c r="L93" s="7"/>
+      <c r="A93" s="10"/>
+      <c r="B93" s="10"/>
+      <c r="C93" s="10"/>
+      <c r="D93" s="11"/>
+      <c r="E93" s="11"/>
+      <c r="F93" s="11"/>
+      <c r="G93" s="11"/>
+      <c r="H93" s="11"/>
+      <c r="I93" s="11"/>
+      <c r="J93" s="11"/>
+      <c r="K93" s="11"/>
+      <c r="L93" s="11"/>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A94" s="21"/>
-      <c r="B94" s="21"/>
-      <c r="C94" s="21"/>
-      <c r="D94" s="7"/>
-      <c r="E94" s="7"/>
-      <c r="F94" s="7"/>
-      <c r="G94" s="7"/>
-      <c r="H94" s="7"/>
-      <c r="I94" s="7"/>
-      <c r="J94" s="7"/>
-      <c r="K94" s="7"/>
-      <c r="L94" s="7"/>
+      <c r="A94" s="10"/>
+      <c r="B94" s="10"/>
+      <c r="C94" s="10"/>
+      <c r="D94" s="11"/>
+      <c r="E94" s="11"/>
+      <c r="F94" s="11"/>
+      <c r="G94" s="11"/>
+      <c r="H94" s="11"/>
+      <c r="I94" s="11"/>
+      <c r="J94" s="11"/>
+      <c r="K94" s="11"/>
+      <c r="L94" s="11"/>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A95" s="21"/>
-      <c r="B95" s="21"/>
-      <c r="C95" s="21"/>
-      <c r="D95" s="7"/>
-      <c r="E95" s="7"/>
-      <c r="F95" s="7"/>
-      <c r="G95" s="7"/>
-      <c r="H95" s="7"/>
-      <c r="I95" s="7"/>
-      <c r="J95" s="7"/>
-      <c r="K95" s="7"/>
-      <c r="L95" s="7"/>
+      <c r="A95" s="10"/>
+      <c r="B95" s="10"/>
+      <c r="C95" s="10"/>
+      <c r="D95" s="11"/>
+      <c r="E95" s="11"/>
+      <c r="F95" s="11"/>
+      <c r="G95" s="11"/>
+      <c r="H95" s="11"/>
+      <c r="I95" s="11"/>
+      <c r="J95" s="11"/>
+      <c r="K95" s="11"/>
+      <c r="L95" s="11"/>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A96" s="21"/>
-      <c r="B96" s="21"/>
-      <c r="C96" s="21"/>
-      <c r="D96" s="7"/>
-      <c r="E96" s="7"/>
-      <c r="F96" s="7"/>
-      <c r="G96" s="7"/>
-      <c r="H96" s="7"/>
-      <c r="I96" s="7"/>
-      <c r="J96" s="7"/>
-      <c r="K96" s="7"/>
-      <c r="L96" s="7"/>
+      <c r="A96" s="10"/>
+      <c r="B96" s="10"/>
+      <c r="C96" s="10"/>
+      <c r="D96" s="11"/>
+      <c r="E96" s="11"/>
+      <c r="F96" s="11"/>
+      <c r="G96" s="11"/>
+      <c r="H96" s="11"/>
+      <c r="I96" s="11"/>
+      <c r="J96" s="11"/>
+      <c r="K96" s="11"/>
+      <c r="L96" s="11"/>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A97" s="21"/>
-      <c r="B97" s="21"/>
-      <c r="C97" s="21"/>
-      <c r="D97" s="7"/>
-      <c r="E97" s="7"/>
-      <c r="F97" s="7"/>
-      <c r="G97" s="7"/>
-      <c r="H97" s="7"/>
-      <c r="I97" s="7"/>
-      <c r="J97" s="7"/>
-      <c r="K97" s="7"/>
-      <c r="L97" s="7"/>
+      <c r="A97" s="10"/>
+      <c r="B97" s="10"/>
+      <c r="C97" s="10"/>
+      <c r="D97" s="11"/>
+      <c r="E97" s="11"/>
+      <c r="F97" s="11"/>
+      <c r="G97" s="11"/>
+      <c r="H97" s="11"/>
+      <c r="I97" s="11"/>
+      <c r="J97" s="11"/>
+      <c r="K97" s="11"/>
+      <c r="L97" s="11"/>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A98" s="21"/>
-      <c r="B98" s="21"/>
-      <c r="C98" s="21"/>
-      <c r="D98" s="7"/>
-      <c r="E98" s="7"/>
-      <c r="F98" s="7"/>
-      <c r="G98" s="7"/>
-      <c r="H98" s="7"/>
-      <c r="I98" s="7"/>
-      <c r="J98" s="7"/>
-      <c r="K98" s="7"/>
-      <c r="L98" s="7"/>
+      <c r="A98" s="10"/>
+      <c r="B98" s="10"/>
+      <c r="C98" s="10"/>
+      <c r="D98" s="11"/>
+      <c r="E98" s="11"/>
+      <c r="F98" s="11"/>
+      <c r="G98" s="11"/>
+      <c r="H98" s="11"/>
+      <c r="I98" s="11"/>
+      <c r="J98" s="11"/>
+      <c r="K98" s="11"/>
+      <c r="L98" s="11"/>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A99" s="21"/>
-      <c r="B99" s="21"/>
-      <c r="C99" s="21"/>
-      <c r="D99" s="7"/>
-      <c r="E99" s="7"/>
-      <c r="F99" s="7"/>
-      <c r="G99" s="7"/>
-      <c r="H99" s="7"/>
-      <c r="I99" s="7"/>
-      <c r="J99" s="7"/>
-      <c r="K99" s="7"/>
-      <c r="L99" s="7"/>
+      <c r="A99" s="10"/>
+      <c r="B99" s="10"/>
+      <c r="C99" s="10"/>
+      <c r="D99" s="11"/>
+      <c r="E99" s="11"/>
+      <c r="F99" s="11"/>
+      <c r="G99" s="11"/>
+      <c r="H99" s="11"/>
+      <c r="I99" s="11"/>
+      <c r="J99" s="11"/>
+      <c r="K99" s="11"/>
+      <c r="L99" s="11"/>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A100" s="21"/>
-      <c r="B100" s="21"/>
-      <c r="C100" s="21"/>
-      <c r="D100" s="7"/>
-      <c r="E100" s="7"/>
-      <c r="F100" s="7"/>
-      <c r="G100" s="7"/>
-      <c r="H100" s="7"/>
-      <c r="I100" s="7"/>
-      <c r="J100" s="7"/>
-      <c r="K100" s="7"/>
-      <c r="L100" s="7"/>
+      <c r="A100" s="10"/>
+      <c r="B100" s="10"/>
+      <c r="C100" s="10"/>
+      <c r="D100" s="11"/>
+      <c r="E100" s="11"/>
+      <c r="F100" s="11"/>
+      <c r="G100" s="11"/>
+      <c r="H100" s="11"/>
+      <c r="I100" s="11"/>
+      <c r="J100" s="11"/>
+      <c r="K100" s="11"/>
+      <c r="L100" s="11"/>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A101" s="21"/>
-      <c r="B101" s="21"/>
-      <c r="C101" s="21"/>
-      <c r="D101" s="7"/>
-      <c r="E101" s="7"/>
-      <c r="F101" s="7"/>
-      <c r="G101" s="7"/>
-      <c r="H101" s="7"/>
-      <c r="I101" s="7"/>
-      <c r="J101" s="7"/>
-      <c r="K101" s="7"/>
-      <c r="L101" s="7"/>
+      <c r="A101" s="10"/>
+      <c r="B101" s="10"/>
+      <c r="C101" s="10"/>
+      <c r="D101" s="11"/>
+      <c r="E101" s="11"/>
+      <c r="F101" s="11"/>
+      <c r="G101" s="11"/>
+      <c r="H101" s="11"/>
+      <c r="I101" s="11"/>
+      <c r="J101" s="11"/>
+      <c r="K101" s="11"/>
+      <c r="L101" s="11"/>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="124"/>
       <c r="B102" s="124"/>
       <c r="C102" s="124"/>
-      <c r="D102" s="8"/>
-      <c r="E102" s="8"/>
-      <c r="F102" s="8"/>
-      <c r="G102" s="8"/>
-      <c r="H102" s="8"/>
-      <c r="I102" s="8"/>
-      <c r="J102" s="8"/>
-      <c r="K102" s="8"/>
-      <c r="L102" s="8"/>
+      <c r="D102" s="121"/>
+      <c r="E102" s="121"/>
+      <c r="F102" s="121"/>
+      <c r="G102" s="121"/>
+      <c r="H102" s="121"/>
+      <c r="I102" s="121"/>
+      <c r="J102" s="121"/>
+      <c r="K102" s="121"/>
+      <c r="L102" s="121"/>
     </row>
     <row r="103" spans="1:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="9" t="s">
+      <c r="A103" s="122" t="s">
         <v>172</v>
       </c>
-      <c r="B103" s="9"/>
-      <c r="C103" s="9"/>
-      <c r="D103" s="10" t="s">
+      <c r="B103" s="122"/>
+      <c r="C103" s="122"/>
+      <c r="D103" s="123" t="s">
         <v>173</v>
       </c>
-      <c r="E103" s="10"/>
-      <c r="F103" s="10"/>
-      <c r="G103" s="10"/>
-      <c r="H103" s="10"/>
-      <c r="I103" s="9" t="s">
+      <c r="E103" s="123"/>
+      <c r="F103" s="123"/>
+      <c r="G103" s="123"/>
+      <c r="H103" s="123"/>
+      <c r="I103" s="122" t="s">
         <v>174</v>
       </c>
-      <c r="J103" s="9"/>
-      <c r="K103" s="9"/>
-      <c r="L103" s="9"/>
+      <c r="J103" s="122"/>
+      <c r="K103" s="122"/>
+      <c r="L103" s="122"/>
     </row>
     <row r="104" spans="1:12" ht="0.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
@@ -7229,25 +7279,201 @@
     </row>
   </sheetData>
   <mergeCells count="240">
-    <mergeCell ref="G2:L2"/>
-    <mergeCell ref="A81:C81"/>
-    <mergeCell ref="D81:G81"/>
-    <mergeCell ref="H81:L81"/>
-    <mergeCell ref="A87:C88"/>
-    <mergeCell ref="I87:L88"/>
-    <mergeCell ref="A89:C90"/>
-    <mergeCell ref="A91:C92"/>
-    <mergeCell ref="A93:C94"/>
-    <mergeCell ref="A95:C96"/>
-    <mergeCell ref="I89:L90"/>
-    <mergeCell ref="I91:L92"/>
-    <mergeCell ref="I93:L94"/>
-    <mergeCell ref="I95:L96"/>
-    <mergeCell ref="D82:H82"/>
-    <mergeCell ref="D83:H84"/>
-    <mergeCell ref="D85:H86"/>
-    <mergeCell ref="D87:H88"/>
-    <mergeCell ref="D89:H90"/>
+    <mergeCell ref="D97:H98"/>
+    <mergeCell ref="D99:H100"/>
+    <mergeCell ref="D101:H102"/>
+    <mergeCell ref="A103:C103"/>
+    <mergeCell ref="D103:H103"/>
+    <mergeCell ref="I103:L103"/>
+    <mergeCell ref="A97:C98"/>
+    <mergeCell ref="A99:C100"/>
+    <mergeCell ref="A101:C102"/>
+    <mergeCell ref="I97:L98"/>
+    <mergeCell ref="I99:L100"/>
+    <mergeCell ref="I101:L102"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="F2:L2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="A82:C82"/>
+    <mergeCell ref="A83:C84"/>
+    <mergeCell ref="B4:D6"/>
+    <mergeCell ref="E4:F6"/>
+    <mergeCell ref="G4:H6"/>
+    <mergeCell ref="I4:K6"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="B7:D8"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="A28:L28"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="A85:C86"/>
+    <mergeCell ref="I82:L82"/>
+    <mergeCell ref="I83:L84"/>
+    <mergeCell ref="I85:L86"/>
+    <mergeCell ref="A9:A17"/>
+    <mergeCell ref="B9:D17"/>
+    <mergeCell ref="E9:F17"/>
+    <mergeCell ref="G9:J12"/>
+    <mergeCell ref="K9:L12"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="A22:E23"/>
+    <mergeCell ref="F22:L23"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="H29:L29"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="H30:L30"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E18:F21"/>
+    <mergeCell ref="G18:L20"/>
+    <mergeCell ref="G21:L21"/>
+    <mergeCell ref="A24:E25"/>
+    <mergeCell ref="F24:L25"/>
+    <mergeCell ref="A26:L27"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="D33:G33"/>
+    <mergeCell ref="H33:L33"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="H34:L34"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="H32:L32"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="D37:G37"/>
+    <mergeCell ref="H37:L37"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="D38:G38"/>
+    <mergeCell ref="H38:L38"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="D35:G35"/>
+    <mergeCell ref="H35:L35"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="D36:G36"/>
+    <mergeCell ref="H36:L36"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="D41:G41"/>
+    <mergeCell ref="H41:L41"/>
+    <mergeCell ref="A42:L42"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="D43:G43"/>
+    <mergeCell ref="H43:L43"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="D39:G39"/>
+    <mergeCell ref="H39:L39"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="D40:G40"/>
+    <mergeCell ref="H40:L40"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="H46:L46"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="D47:G47"/>
+    <mergeCell ref="H47:L47"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="D44:G44"/>
+    <mergeCell ref="H44:L44"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="D45:G45"/>
+    <mergeCell ref="H45:L45"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="D50:G50"/>
+    <mergeCell ref="H50:L50"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="D51:G51"/>
+    <mergeCell ref="H51:L51"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="D48:G48"/>
+    <mergeCell ref="H48:L48"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="D49:G49"/>
+    <mergeCell ref="H49:L49"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="D54:G54"/>
+    <mergeCell ref="H54:L54"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="D55:G55"/>
+    <mergeCell ref="H55:L55"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="D52:G52"/>
+    <mergeCell ref="H52:L52"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="D53:G53"/>
+    <mergeCell ref="H53:L53"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="D58:G58"/>
+    <mergeCell ref="H58:L58"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="D59:G59"/>
+    <mergeCell ref="H59:L59"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="D56:G56"/>
+    <mergeCell ref="H56:L56"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="D57:G57"/>
+    <mergeCell ref="H57:L57"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="D62:G62"/>
+    <mergeCell ref="H62:L62"/>
+    <mergeCell ref="A63:L63"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="D64:G64"/>
+    <mergeCell ref="H64:L64"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="D60:G60"/>
+    <mergeCell ref="H60:L60"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="D61:G61"/>
+    <mergeCell ref="H61:L61"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="D67:G67"/>
+    <mergeCell ref="H67:L67"/>
+    <mergeCell ref="A68:C68"/>
+    <mergeCell ref="D68:G68"/>
+    <mergeCell ref="H68:L68"/>
+    <mergeCell ref="A65:C65"/>
+    <mergeCell ref="D65:G65"/>
+    <mergeCell ref="H65:L65"/>
+    <mergeCell ref="A66:C66"/>
+    <mergeCell ref="D66:G66"/>
+    <mergeCell ref="H66:L66"/>
+    <mergeCell ref="H74:L74"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="D71:G71"/>
+    <mergeCell ref="H71:L71"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="D72:G72"/>
+    <mergeCell ref="H72:L72"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="D69:G69"/>
+    <mergeCell ref="H69:L69"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="D70:G70"/>
+    <mergeCell ref="H70:L70"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A79:C79"/>
     <mergeCell ref="D79:G79"/>
@@ -7272,203 +7498,27 @@
     <mergeCell ref="H73:L73"/>
     <mergeCell ref="A74:C74"/>
     <mergeCell ref="D74:G74"/>
-    <mergeCell ref="H74:L74"/>
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="D71:G71"/>
-    <mergeCell ref="H71:L71"/>
-    <mergeCell ref="A72:C72"/>
-    <mergeCell ref="D72:G72"/>
-    <mergeCell ref="H72:L72"/>
-    <mergeCell ref="A69:C69"/>
-    <mergeCell ref="D69:G69"/>
-    <mergeCell ref="H69:L69"/>
-    <mergeCell ref="A70:C70"/>
-    <mergeCell ref="D70:G70"/>
-    <mergeCell ref="H70:L70"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="D67:G67"/>
-    <mergeCell ref="H67:L67"/>
-    <mergeCell ref="A68:C68"/>
-    <mergeCell ref="D68:G68"/>
-    <mergeCell ref="H68:L68"/>
-    <mergeCell ref="A65:C65"/>
-    <mergeCell ref="D65:G65"/>
-    <mergeCell ref="H65:L65"/>
-    <mergeCell ref="A66:C66"/>
-    <mergeCell ref="D66:G66"/>
-    <mergeCell ref="H66:L66"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="D62:G62"/>
-    <mergeCell ref="H62:L62"/>
-    <mergeCell ref="A63:L63"/>
-    <mergeCell ref="A64:C64"/>
-    <mergeCell ref="D64:G64"/>
-    <mergeCell ref="H64:L64"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="D60:G60"/>
-    <mergeCell ref="H60:L60"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="D61:G61"/>
-    <mergeCell ref="H61:L61"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="D58:G58"/>
-    <mergeCell ref="H58:L58"/>
-    <mergeCell ref="A59:C59"/>
-    <mergeCell ref="D59:G59"/>
-    <mergeCell ref="H59:L59"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="D56:G56"/>
-    <mergeCell ref="H56:L56"/>
-    <mergeCell ref="A57:C57"/>
-    <mergeCell ref="D57:G57"/>
-    <mergeCell ref="H57:L57"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="D54:G54"/>
-    <mergeCell ref="H54:L54"/>
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="D55:G55"/>
-    <mergeCell ref="H55:L55"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="D52:G52"/>
-    <mergeCell ref="H52:L52"/>
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="D53:G53"/>
-    <mergeCell ref="H53:L53"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="D50:G50"/>
-    <mergeCell ref="H50:L50"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="D51:G51"/>
-    <mergeCell ref="H51:L51"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="D48:G48"/>
-    <mergeCell ref="H48:L48"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="D49:G49"/>
-    <mergeCell ref="H49:L49"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="D46:G46"/>
-    <mergeCell ref="H46:L46"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="D47:G47"/>
-    <mergeCell ref="H47:L47"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="D44:G44"/>
-    <mergeCell ref="H44:L44"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="D45:G45"/>
-    <mergeCell ref="H45:L45"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="D41:G41"/>
-    <mergeCell ref="H41:L41"/>
-    <mergeCell ref="A42:L42"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="D43:G43"/>
-    <mergeCell ref="H43:L43"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="D39:G39"/>
-    <mergeCell ref="H39:L39"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="D40:G40"/>
-    <mergeCell ref="H40:L40"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="D37:G37"/>
-    <mergeCell ref="H37:L37"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="D38:G38"/>
-    <mergeCell ref="H38:L38"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="D35:G35"/>
-    <mergeCell ref="H35:L35"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="D36:G36"/>
-    <mergeCell ref="H36:L36"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="D33:G33"/>
-    <mergeCell ref="H33:L33"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="D34:G34"/>
-    <mergeCell ref="H34:L34"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="H32:L32"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="H29:L29"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="H30:L30"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E18:F21"/>
-    <mergeCell ref="G18:L20"/>
-    <mergeCell ref="G21:L21"/>
-    <mergeCell ref="A24:E25"/>
-    <mergeCell ref="F24:L25"/>
-    <mergeCell ref="A26:L27"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="H31:L31"/>
-    <mergeCell ref="A85:C86"/>
-    <mergeCell ref="I82:L82"/>
-    <mergeCell ref="I83:L84"/>
-    <mergeCell ref="I85:L86"/>
-    <mergeCell ref="A9:A17"/>
-    <mergeCell ref="B9:D17"/>
-    <mergeCell ref="E9:F17"/>
-    <mergeCell ref="G9:J12"/>
-    <mergeCell ref="K9:L12"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="A22:E23"/>
-    <mergeCell ref="F22:L23"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="A82:C82"/>
-    <mergeCell ref="A83:C84"/>
-    <mergeCell ref="B4:D6"/>
-    <mergeCell ref="E4:F6"/>
-    <mergeCell ref="G4:H6"/>
-    <mergeCell ref="I4:K6"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="B7:D8"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="A28:L28"/>
-    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="A81:C81"/>
+    <mergeCell ref="D81:G81"/>
+    <mergeCell ref="H81:L81"/>
+    <mergeCell ref="A87:C88"/>
+    <mergeCell ref="I87:L88"/>
+    <mergeCell ref="A89:C90"/>
+    <mergeCell ref="A91:C92"/>
+    <mergeCell ref="A93:C94"/>
+    <mergeCell ref="A95:C96"/>
+    <mergeCell ref="I89:L90"/>
+    <mergeCell ref="I91:L92"/>
+    <mergeCell ref="I93:L94"/>
+    <mergeCell ref="I95:L96"/>
+    <mergeCell ref="D82:H82"/>
+    <mergeCell ref="D83:H84"/>
+    <mergeCell ref="D85:H86"/>
+    <mergeCell ref="D87:H88"/>
+    <mergeCell ref="D89:H90"/>
     <mergeCell ref="D91:H92"/>
     <mergeCell ref="D93:H94"/>
     <mergeCell ref="D95:H96"/>
-    <mergeCell ref="D97:H98"/>
-    <mergeCell ref="D99:H100"/>
-    <mergeCell ref="D101:H102"/>
-    <mergeCell ref="A103:C103"/>
-    <mergeCell ref="D103:H103"/>
-    <mergeCell ref="I103:L103"/>
-    <mergeCell ref="A97:C98"/>
-    <mergeCell ref="A99:C100"/>
-    <mergeCell ref="A101:C102"/>
-    <mergeCell ref="I97:L98"/>
-    <mergeCell ref="I99:L100"/>
-    <mergeCell ref="I101:L102"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="75" orientation="portrait" r:id="rId1"/>

</xml_diff>